<commit_message>
Small changes to test data
</commit_message>
<xml_diff>
--- a/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
+++ b/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\eclipse-workspace\ddsdet137\DsAlgoAvengers\src\test\resources\com\dsalgoproject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1BB0C4-F755-42C3-B833-2883E9656993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D2DC55-ABCB-453F-A233-7BC92AF6CD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{41B4179E-F2E0-4E6C-861D-46A636914020}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{41B4179E-F2E0-4E6C-861D-46A636914020}"/>
   </bookViews>
   <sheets>
     <sheet name="registerValidUserSheet" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>answer</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Qwerty#123</t>
   </si>
   <si>
-    <t>Qwerty)123</t>
-  </si>
-  <si>
     <t>Testing+123</t>
   </si>
   <si>
@@ -185,12 +182,6 @@
   </si>
   <si>
     <t>expectedOutput</t>
-  </si>
-  <si>
-    <t>testuserAvengers3</t>
-  </si>
-  <si>
-    <t>Qwerty+123458</t>
   </si>
   <si>
     <t>def findMaxConsecutiveOnes(nums) :
@@ -255,6 +246,12 @@
   return squared
 nums = [-7,-3,2,3,11]
 print(sortedSquares(nums))</t>
+  </si>
+  <si>
+    <t>testuserAvengers35</t>
+  </si>
+  <si>
+    <t>Qwerty+1234586</t>
   </si>
 </sst>
 </file>
@@ -623,15 +620,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -642,37 +639,37 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A2)</f>
-        <v>New Account Created. You are logged in as testuserAvengers3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>New Account Created. You are logged in as testuserAvengers35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A3)</f>
-        <v>New Account Created. You are logged in as Qwerty+123458</v>
+        <v>New Account Created. You are logged in as Qwerty+1234586</v>
       </c>
     </row>
   </sheetData>
@@ -684,21 +681,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02E924F-A23B-4E63-ABF4-137A81ECC818}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -709,24 +706,24 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -734,38 +731,24 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -782,15 +765,15 @@
       <selection activeCell="E20" sqref="E9:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -804,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -818,7 +801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -832,12 +815,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="216" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -846,12 +829,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>18</v>
@@ -860,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -874,7 +857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -888,12 +871,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -902,12 +885,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update excel to pract ques
</commit_message>
<xml_diff>
--- a/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
+++ b/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\eclipse-workspace\ddsdet137\DsAlgoAvengers\src\test\resources\com\dsalgoproject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D2DC55-ABCB-453F-A233-7BC92AF6CD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C76C90-476A-4352-A5FF-60AFC59BBA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{41B4179E-F2E0-4E6C-861D-46A636914020}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41B4179E-F2E0-4E6C-861D-46A636914020}"/>
   </bookViews>
   <sheets>
     <sheet name="registerValidUserSheet" sheetId="2" r:id="rId1"/>
@@ -248,10 +248,10 @@
 print(sortedSquares(nums))</t>
   </si>
   <si>
-    <t>testuserAvengers35</t>
-  </si>
-  <si>
-    <t>Qwerty+1234586</t>
+    <t>testuserAvengers55</t>
+  </si>
+  <si>
+    <t>Qwerty+123458787</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F75C092-D528-4B80-8D1C-1E6C3C64B167}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="122" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -654,7 +654,7 @@
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A2)</f>
-        <v>New Account Created. You are logged in as testuserAvengers35</v>
+        <v>New Account Created. You are logged in as testuserAvengers55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A3)</f>
-        <v>New Account Created. You are logged in as Qwerty+1234586</v>
+        <v>New Account Created. You are logged in as Qwerty+123458787</v>
       </c>
     </row>
   </sheetData>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE84CAB-1B89-4A14-8D18-46466C0ACD0D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E20" sqref="E9:E20"/>
+    <sheetView zoomScale="78" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,11 +787,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -801,11 +801,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">

</xml_diff>

<commit_message>
new test data for valid regis
</commit_message>
<xml_diff>
--- a/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
+++ b/src/test/resources/com/dsalgoproject/testData/dsAlgoTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\eclipse-workspace\ddsdet137\DsAlgoAvengers\src\test\resources\com\dsalgoproject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70975128-F8F0-457E-AF57-336B4084C833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D866670-8BF9-4E13-97C2-044BC0EDB521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41B4179E-F2E0-4E6C-861D-46A636914020}"/>
   </bookViews>
@@ -248,10 +248,10 @@
 print(sortedSquares(nums))</t>
   </si>
   <si>
-    <t>testuserAvengers56</t>
-  </si>
-  <si>
-    <t>Qwerty+1234587809</t>
+    <t>testuserAvengers989</t>
+  </si>
+  <si>
+    <t>Qwerty+12345878889</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +654,7 @@
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A2)</f>
-        <v>New Account Created. You are logged in as testuserAvengers56</v>
+        <v>New Account Created. You are logged in as testuserAvengers989</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("New Account Created. You are logged in as ",A3)</f>
-        <v>New Account Created. You are logged in as Qwerty+1234587809</v>
+        <v>New Account Created. You are logged in as Qwerty+12345878889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>